<commit_message>
Add Inventory (only design)
</commit_message>
<xml_diff>
--- a/Labyrinthe.xlsx
+++ b/Labyrinthe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximef\Desktop\1ARC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megaport\Desktop\1ARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AEE822-B53F-4964-901C-7C5D5DE5FB8C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4F06A4-A366-411B-BDE1-02C941F5201A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="17">
   <si>
     <t>DD</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>*message*</t>
-  </si>
-  <si>
-    <t>Press</t>
   </si>
   <si>
     <t>═</t>
@@ -183,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,6 +222,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="BZ10" sqref="BZ10"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
+      <selection activeCell="BN7" sqref="BN7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -557,189 +557,191 @@
         <v>2</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="S1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="AJ1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="AP1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="T1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="U1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="V1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="X1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AJ1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AP1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AT1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AU1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AV1" s="11" t="s">
-        <v>6</v>
-      </c>
       <c r="AW1" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AX1" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AY1" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AZ1" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BA1" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BB1" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BC1" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BD1" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BE1" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BF1" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BG1" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BH1" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BI1" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="BJ1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="BK1" s="13"/>
+        <v>2</v>
+      </c>
+      <c r="BK1" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="BL1" s="13"/>
       <c r="BM1" s="13"/>
       <c r="BN1" s="13"/>
@@ -747,11 +749,13 @@
       <c r="BP1" s="13"/>
       <c r="BQ1" s="13"/>
       <c r="BR1" s="13"/>
-      <c r="BS1" s="13"/>
+      <c r="BS1" s="11"/>
       <c r="BT1" s="13"/>
-      <c r="BU1" s="13"/>
-      <c r="BV1" s="13"/>
-      <c r="BW1" s="13"/>
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11"/>
+      <c r="BW1" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="BX1" s="13"/>
       <c r="BY1" s="13"/>
       <c r="BZ1" s="13"/>
@@ -766,7 +770,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -784,7 +788,7 @@
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
       <c r="R2" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S2" s="10"/>
       <c r="T2" s="13"/>
@@ -803,7 +807,7 @@
       <c r="AG2" s="10"/>
       <c r="AH2" s="10"/>
       <c r="AI2" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AJ2" s="12"/>
       <c r="AK2" s="12"/>
@@ -811,7 +815,7 @@
       <c r="AM2" s="10"/>
       <c r="AN2" s="10"/>
       <c r="AO2" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AP2" s="13"/>
       <c r="AQ2" s="13"/>
@@ -820,7 +824,7 @@
       <c r="AT2" s="13"/>
       <c r="AU2" s="13"/>
       <c r="AV2" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AW2" s="10"/>
       <c r="AX2" s="10"/>
@@ -837,10 +841,14 @@
         <v>0</v>
       </c>
       <c r="BI2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="BJ2" s="10"/>
-      <c r="BK2" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="BJ2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK2" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="BL2" s="13"/>
       <c r="BM2" s="13"/>
       <c r="BN2" s="13"/>
@@ -848,11 +856,13 @@
       <c r="BP2" s="13"/>
       <c r="BQ2" s="13"/>
       <c r="BR2" s="13"/>
-      <c r="BS2" s="13"/>
+      <c r="BS2" s="11"/>
       <c r="BT2" s="13"/>
-      <c r="BU2" s="13"/>
-      <c r="BV2" s="13"/>
-      <c r="BW2" s="13"/>
+      <c r="BU2" s="11"/>
+      <c r="BV2" s="11"/>
+      <c r="BW2" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="BX2" s="13"/>
       <c r="BY2" s="13"/>
       <c r="BZ2" s="13"/>
@@ -867,161 +877,165 @@
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" s="11"/>
       <c r="K3" s="13"/>
       <c r="L3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O3" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P3" s="13"/>
       <c r="Q3" s="13"/>
       <c r="R3" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="S3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="X3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="T3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="U3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="V3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="W3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="X3" s="11" t="s">
-        <v>6</v>
-      </c>
       <c r="Y3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Z3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AB3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AD3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AF3" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AG3" s="10"/>
       <c r="AH3" s="10"/>
       <c r="AI3" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AJ3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AK3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AL3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AM3" s="10"/>
       <c r="AN3" s="10"/>
       <c r="AO3" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AP3" s="10"/>
       <c r="AQ3" s="10"/>
       <c r="AR3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AS3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AT3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AU3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AV3" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AW3" s="10"/>
       <c r="AX3" s="10"/>
       <c r="AY3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AZ3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BA3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BB3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BC3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BD3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BE3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BF3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BG3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BH3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BI3" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="BJ3" s="10"/>
-      <c r="BK3" s="13"/>
+        <v>12</v>
+      </c>
+      <c r="BJ3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK3" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="BL3" s="13"/>
       <c r="BM3" s="13"/>
       <c r="BN3" s="13"/>
@@ -1029,11 +1043,13 @@
       <c r="BP3" s="13"/>
       <c r="BQ3" s="13"/>
       <c r="BR3" s="13"/>
-      <c r="BS3" s="13"/>
+      <c r="BS3" s="11"/>
       <c r="BT3" s="13"/>
-      <c r="BU3" s="13"/>
-      <c r="BV3" s="13"/>
-      <c r="BW3" s="13"/>
+      <c r="BU3" s="11"/>
+      <c r="BV3" s="11"/>
+      <c r="BW3" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="BX3" s="13"/>
       <c r="BY3" s="13"/>
       <c r="BZ3" s="13"/>
@@ -1048,7 +1064,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -1057,7 +1073,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
@@ -1065,7 +1081,7 @@
       <c r="M4" s="13"/>
       <c r="N4" s="10"/>
       <c r="O4" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P4" s="13"/>
       <c r="Q4" s="10"/>
@@ -1076,7 +1092,7 @@
       <c r="V4" s="10"/>
       <c r="W4" s="13"/>
       <c r="X4" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y4" s="11"/>
       <c r="Z4" s="11"/>
@@ -1086,7 +1102,7 @@
       <c r="AD4" s="11"/>
       <c r="AE4" s="12"/>
       <c r="AF4" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AG4" s="10"/>
       <c r="AH4" s="10"/>
@@ -1097,7 +1113,7 @@
       <c r="AM4" s="10"/>
       <c r="AN4" s="10"/>
       <c r="AO4" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AP4" s="10"/>
       <c r="AQ4" s="10"/>
@@ -1106,7 +1122,7 @@
       <c r="AT4" s="13"/>
       <c r="AU4" s="13"/>
       <c r="AV4" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AW4" s="10"/>
       <c r="AX4" s="10"/>
@@ -1121,22 +1137,38 @@
       <c r="BG4" s="10"/>
       <c r="BH4" s="10"/>
       <c r="BI4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="BJ4" s="10"/>
-      <c r="BK4" s="13"/>
-      <c r="BL4" s="13"/>
-      <c r="BM4" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="BJ4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="BL4" s="15"/>
+      <c r="BM4" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="BN4" s="13"/>
-      <c r="BO4" s="13"/>
+      <c r="BO4" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="BP4" s="13"/>
-      <c r="BQ4" s="13"/>
+      <c r="BQ4" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="BR4" s="13"/>
-      <c r="BS4" s="13"/>
-      <c r="BT4" s="13"/>
-      <c r="BU4" s="13"/>
-      <c r="BV4" s="13"/>
-      <c r="BW4" s="13"/>
+      <c r="BS4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="BT4" s="11"/>
+      <c r="BU4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BV4" s="11"/>
+      <c r="BW4" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="BX4" s="13"/>
       <c r="BY4" s="13"/>
       <c r="BZ4" s="13"/>
@@ -1151,163 +1183,191 @@
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M5" s="11"/>
       <c r="N5" s="10"/>
       <c r="O5" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="V5" s="11"/>
       <c r="W5" s="11"/>
       <c r="X5" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y5" s="10"/>
       <c r="Z5" s="11"/>
       <c r="AA5" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AB5" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AC5" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AD5" s="10"/>
       <c r="AE5" s="11"/>
       <c r="AF5" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AG5" s="10"/>
       <c r="AH5" s="10"/>
       <c r="AI5" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AJ5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AK5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AL5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AM5" s="10"/>
       <c r="AN5" s="13"/>
       <c r="AO5" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AP5" s="13"/>
       <c r="AQ5" s="13"/>
       <c r="AR5" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AS5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AT5" s="10"/>
       <c r="AU5" s="11"/>
       <c r="AV5" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AW5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AX5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AY5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AZ5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BA5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BB5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BC5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BD5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BE5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BF5" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BG5" s="10"/>
       <c r="BH5" s="10"/>
       <c r="BI5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="BJ5" s="10"/>
-      <c r="BK5" s="13"/>
-      <c r="BL5" s="13"/>
-      <c r="BM5" s="13"/>
-      <c r="BN5" s="13"/>
-      <c r="BO5" s="13"/>
-      <c r="BP5" s="13"/>
-      <c r="BQ5" s="13"/>
-      <c r="BR5" s="13"/>
-      <c r="BS5" s="13"/>
-      <c r="BT5" s="13"/>
-      <c r="BU5" s="13"/>
-      <c r="BV5" s="13"/>
-      <c r="BW5" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="BJ5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="BK5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="BL5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BM5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BN5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BO5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BP5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BQ5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BR5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BT5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BU5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BV5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BW5" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="BX5" s="13"/>
       <c r="BY5" s="13"/>
       <c r="BZ5" s="13"/>
@@ -1322,7 +1382,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -1343,7 +1403,7 @@
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
       <c r="U6" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="10"/>
@@ -1353,23 +1413,23 @@
       <c r="Y6" s="13"/>
       <c r="Z6" s="13"/>
       <c r="AA6" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AB6" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AC6" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AD6" s="11"/>
       <c r="AE6" s="11"/>
       <c r="AF6" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AG6" s="10"/>
       <c r="AH6" s="10"/>
       <c r="AI6" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AJ6" s="10"/>
       <c r="AK6" s="10"/>
@@ -1377,12 +1437,12 @@
       <c r="AM6" s="10"/>
       <c r="AN6" s="11"/>
       <c r="AO6" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AP6" s="10"/>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AS6" s="13"/>
       <c r="AT6" s="13"/>
@@ -1401,7 +1461,7 @@
       <c r="BG6" s="13"/>
       <c r="BH6" s="13"/>
       <c r="BI6" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ6" s="10" t="s">
         <v>3</v>
@@ -1433,152 +1493,152 @@
         <v>2</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>6</v>
-      </c>
       <c r="P7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X7" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
       <c r="AA7" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB7" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AC7" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AD7" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AE7" s="11"/>
       <c r="AF7" s="10"/>
       <c r="AG7" s="10"/>
       <c r="AH7" s="10"/>
       <c r="AI7" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AJ7" s="10"/>
       <c r="AK7" s="10"/>
       <c r="AL7" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AM7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AN7" s="11" t="s">
-        <v>6</v>
-      </c>
       <c r="AO7" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AP7" s="10"/>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AS7" s="13"/>
       <c r="AT7" s="11"/>
       <c r="AU7" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AV7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AW7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AX7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AY7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AZ7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BA7" s="10"/>
       <c r="BB7" s="10"/>
       <c r="BC7" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="BD7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BE7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BF7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BG7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BH7" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BI7" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BJ7" s="10" t="s">
         <v>3</v>
@@ -1610,7 +1670,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -1625,7 +1685,7 @@
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
@@ -1636,7 +1696,7 @@
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
       <c r="X8" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="10"/>
@@ -1644,44 +1704,44 @@
       <c r="AB8" s="10"/>
       <c r="AC8" s="10"/>
       <c r="AD8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI8" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="AE8" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF8" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH8" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI8" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="AJ8" s="10"/>
       <c r="AK8" s="10"/>
       <c r="AL8" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AM8" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AN8" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AO8" s="12"/>
       <c r="AP8" s="11"/>
       <c r="AQ8" s="11"/>
       <c r="AR8" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AS8" s="13"/>
       <c r="AT8" s="13"/>
       <c r="AU8" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AV8" s="13"/>
       <c r="AW8" s="13"/>
@@ -1691,7 +1751,7 @@
       <c r="BA8" s="10"/>
       <c r="BB8" s="10"/>
       <c r="BC8" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BD8" s="10"/>
       <c r="BE8" s="10"/>
@@ -1699,7 +1759,7 @@
       <c r="BG8" s="10"/>
       <c r="BH8" s="10"/>
       <c r="BI8" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ8" s="10"/>
       <c r="BK8" s="13"/>
@@ -1729,62 +1789,62 @@
         <v>2</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="11"/>
       <c r="O9" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
       <c r="U9" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
       <c r="X9" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y9" s="10"/>
       <c r="Z9" s="10"/>
       <c r="AA9" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AB9" s="10"/>
       <c r="AC9" s="10"/>
@@ -1792,7 +1852,7 @@
       <c r="AE9" s="10"/>
       <c r="AF9" s="10"/>
       <c r="AG9" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AH9" s="13"/>
       <c r="AI9" s="13"/>
@@ -1801,58 +1861,58 @@
       <c r="AL9" s="11"/>
       <c r="AM9" s="10"/>
       <c r="AN9" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AO9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AP9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AQ9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AR9" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AS9" s="13"/>
       <c r="AT9" s="13"/>
       <c r="AU9" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AV9" s="11"/>
       <c r="AW9" s="11"/>
       <c r="AX9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AY9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AZ9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BA9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BB9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BC9" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="BD9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BE9" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BF9" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="BG9" s="10"/>
       <c r="BH9" s="10"/>
       <c r="BI9" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ9" s="10"/>
       <c r="BK9" s="13"/>
@@ -1882,19 +1942,19 @@
         <v>2</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -1910,53 +1970,53 @@
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
       <c r="U10" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
       <c r="X10" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y10" s="10"/>
       <c r="Z10" s="10"/>
       <c r="AA10" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AB10" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC10" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AD10" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AE10" s="10"/>
       <c r="AF10" s="10"/>
       <c r="AG10" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AH10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AI10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ10" s="11" t="s">
-        <v>6</v>
-      </c>
       <c r="AK10" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AL10" s="11"/>
       <c r="AM10" s="10"/>
       <c r="AN10" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AO10" s="13"/>
       <c r="AP10" s="10"/>
@@ -1965,7 +2025,7 @@
       <c r="AS10" s="10"/>
       <c r="AT10" s="13"/>
       <c r="AU10" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AV10" s="12"/>
       <c r="AW10" s="12"/>
@@ -1978,12 +2038,12 @@
       <c r="BD10" s="10"/>
       <c r="BE10" s="10"/>
       <c r="BF10" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BG10" s="10"/>
       <c r="BH10" s="10"/>
       <c r="BI10" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ10" s="10"/>
       <c r="BK10" s="13"/>
@@ -2013,61 +2073,61 @@
         <v>2</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="10"/>
       <c r="I11" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="L11" s="11" t="s">
-        <v>6</v>
-      </c>
       <c r="M11" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N11" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q11" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R11" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S11" s="11"/>
       <c r="T11" s="11"/>
       <c r="U11" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V11" s="13"/>
       <c r="W11" s="13"/>
       <c r="X11" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10"/>
@@ -2075,7 +2135,7 @@
       <c r="AB11" s="10"/>
       <c r="AC11" s="10"/>
       <c r="AD11" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AE11" s="10"/>
       <c r="AF11" s="10"/>
@@ -2083,68 +2143,68 @@
       <c r="AH11" s="10"/>
       <c r="AI11" s="10"/>
       <c r="AJ11" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AK11" s="10"/>
       <c r="AL11" s="11"/>
       <c r="AM11" s="10"/>
       <c r="AN11" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AO11" s="13"/>
       <c r="AP11" s="10"/>
       <c r="AQ11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY11" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="AR11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AT11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AU11" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="AV11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AW11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AX11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AY11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AZ11" s="11" t="s">
-        <v>6</v>
-      </c>
       <c r="BA11" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BB11" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BC11" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BD11" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BE11" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BF11" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="BG11" s="10"/>
       <c r="BH11" s="10"/>
       <c r="BI11" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ11" s="10"/>
       <c r="BK11" s="13"/>
@@ -2174,7 +2234,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
@@ -2183,76 +2243,76 @@
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
       <c r="L12" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="7" t="s">
         <v>1</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="6" t="s">
         <v>1</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
       <c r="U12" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="V12" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="W12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="W12" s="11" t="s">
-        <v>6</v>
-      </c>
       <c r="X12" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Y12" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Z12" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA12" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AB12" s="10"/>
       <c r="AC12" s="10"/>
       <c r="AD12" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AE12" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AF12" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AG12" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AH12" s="10"/>
       <c r="AI12" s="10"/>
       <c r="AJ12" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AK12" s="11"/>
       <c r="AL12" s="11"/>
       <c r="AM12" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AN12" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AO12" s="13"/>
       <c r="AP12" s="10"/>
@@ -2266,7 +2326,7 @@
       <c r="AX12" s="10"/>
       <c r="AY12" s="10"/>
       <c r="AZ12" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BA12" s="13"/>
       <c r="BB12" s="13"/>
@@ -2277,7 +2337,7 @@
       <c r="BG12" s="13"/>
       <c r="BH12" s="13"/>
       <c r="BI12" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ12" s="10"/>
       <c r="BK12" s="13"/>
@@ -2307,15 +2367,15 @@
         <v>2</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -2323,24 +2383,24 @@
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
       <c r="L13" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
       <c r="R13" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S13" s="11"/>
       <c r="T13" s="11"/>
       <c r="U13" s="12"/>
       <c r="V13" s="10"/>
       <c r="W13" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X13" s="13"/>
       <c r="Y13" s="10"/>
@@ -2349,48 +2409,48 @@
       <c r="AB13" s="10"/>
       <c r="AC13" s="10"/>
       <c r="AD13" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AE13" s="10"/>
       <c r="AF13" s="10"/>
       <c r="AG13" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AH13" s="10"/>
       <c r="AI13" s="10"/>
       <c r="AJ13" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AK13" s="13"/>
       <c r="AL13" s="8" t="s">
         <v>1</v>
       </c>
       <c r="AM13" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AN13" s="13"/>
       <c r="AO13" s="13"/>
       <c r="AP13" s="10"/>
       <c r="AQ13" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AR13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AS13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AT13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AU13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AV13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AW13" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AX13" s="13"/>
       <c r="AY13" s="11"/>
@@ -2398,21 +2458,21 @@
       <c r="BA13" s="10"/>
       <c r="BB13" s="10"/>
       <c r="BC13" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="BD13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BE13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BF13" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BG13" s="10"/>
       <c r="BH13" s="10"/>
       <c r="BI13" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ13" s="10"/>
       <c r="BK13" s="13"/>
@@ -2442,98 +2502,98 @@
         <v>2</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="L14" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="S14" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T14" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U14" s="11"/>
       <c r="V14" s="10"/>
       <c r="W14" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X14" s="13"/>
       <c r="Y14" s="10"/>
       <c r="Z14" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA14" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AB14" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC14" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AD14" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AE14" s="10"/>
       <c r="AF14" s="10"/>
       <c r="AG14" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AH14" s="10"/>
       <c r="AI14" s="10"/>
       <c r="AJ14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AK14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM14" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="AK14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM14" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="AN14" s="10"/>
       <c r="AO14" s="10"/>
       <c r="AP14" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AQ14" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AR14" s="13"/>
       <c r="AS14" s="10"/>
@@ -2541,25 +2601,25 @@
       <c r="AU14" s="11"/>
       <c r="AV14" s="11"/>
       <c r="AW14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB14" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC14" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="AX14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AY14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AZ14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="BA14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="BB14" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="BC14" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="BD14" s="10"/>
       <c r="BE14" s="10"/>
@@ -2567,7 +2627,7 @@
       <c r="BG14" s="10"/>
       <c r="BH14" s="10"/>
       <c r="BI14" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ14" s="10"/>
       <c r="BK14" s="13"/>
@@ -2597,7 +2657,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
@@ -2612,7 +2672,7 @@
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
@@ -2622,7 +2682,7 @@
       <c r="U15" s="10"/>
       <c r="V15" s="10"/>
       <c r="W15" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X15" s="13"/>
       <c r="Y15" s="10"/>
@@ -2634,7 +2694,7 @@
       <c r="AE15" s="10"/>
       <c r="AF15" s="10"/>
       <c r="AG15" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AH15" s="10"/>
       <c r="AI15" s="10"/>
@@ -2645,13 +2705,13 @@
       <c r="AN15" s="10"/>
       <c r="AO15" s="10"/>
       <c r="AP15" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="10"/>
       <c r="AS15" s="10"/>
       <c r="AT15" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AU15" s="10"/>
       <c r="AV15" s="10"/>
@@ -2665,16 +2725,16 @@
       <c r="BD15" s="10"/>
       <c r="BE15" s="13"/>
       <c r="BF15" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="BG15" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BH15" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BI15" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="BJ15" s="10"/>
       <c r="BK15" s="13"/>
@@ -2704,166 +2764,166 @@
         <v>2</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="J16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="O16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="N16" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="O16" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="P16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q16" s="11" t="s">
-        <v>6</v>
-      </c>
       <c r="R16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="U16" s="13"/>
       <c r="V16" s="10"/>
       <c r="W16" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="10"/>
       <c r="Z16" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AA16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AB16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AD16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AF16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AG16" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AH16" s="10"/>
       <c r="AI16" s="10"/>
       <c r="AJ16" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AK16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AL16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AM16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AN16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AO16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AP16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="AQ16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AT16" s="12" t="s">
-        <v>15</v>
-      </c>
       <c r="AU16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AV16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AW16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AX16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AY16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AZ16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BA16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BB16" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BC16" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="BD16" s="10"/>
       <c r="BE16" s="10"/>
       <c r="BF16" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BG16" s="10"/>
       <c r="BH16" s="9" t="s">
         <v>1</v>
       </c>
       <c r="BI16" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ16" s="10"/>
       <c r="BK16" s="13"/>
@@ -2893,7 +2953,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -2902,7 +2962,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
@@ -2914,22 +2974,22 @@
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
       <c r="Q17" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R17" s="11"/>
       <c r="S17" s="13"/>
       <c r="T17" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U17" s="13"/>
       <c r="V17" s="10"/>
       <c r="W17" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="10"/>
       <c r="Z17" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA17" s="11"/>
       <c r="AB17" s="13"/>
@@ -2941,7 +3001,7 @@
       <c r="AH17" s="10"/>
       <c r="AI17" s="10"/>
       <c r="AJ17" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AK17" s="10"/>
       <c r="AL17" s="10"/>
@@ -2953,7 +3013,7 @@
       <c r="AR17" s="10"/>
       <c r="AS17" s="10"/>
       <c r="AT17" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AU17" s="10"/>
       <c r="AV17" s="10"/>
@@ -2964,17 +3024,17 @@
       <c r="BA17" s="10"/>
       <c r="BB17" s="10"/>
       <c r="BC17" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BD17" s="10"/>
       <c r="BE17" s="10"/>
       <c r="BF17" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BG17" s="10"/>
       <c r="BH17" s="10"/>
       <c r="BI17" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ17" s="10"/>
       <c r="BK17" s="13"/>
@@ -3004,136 +3064,136 @@
         <v>2</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="10"/>
       <c r="I18" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
       <c r="L18" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M18" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
       <c r="Q18" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="R18" s="11"/>
       <c r="S18" s="13"/>
       <c r="T18" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U18" s="13"/>
       <c r="V18" s="10"/>
       <c r="W18" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="X18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Z18" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AA18" s="11"/>
       <c r="AB18" s="10"/>
       <c r="AC18" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AD18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AF18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AG18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AI18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AJ18" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AK18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AL18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AM18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AN18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AO18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AP18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AQ18" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AR18" s="10"/>
       <c r="AS18" s="10"/>
       <c r="AT18" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AU18" s="10"/>
       <c r="AV18" s="11"/>
       <c r="AW18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AX18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AY18" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AZ18" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="BA18" s="10"/>
       <c r="BB18" s="10"/>
       <c r="BC18" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BD18" s="10"/>
       <c r="BE18" s="10"/>
       <c r="BF18" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BG18" s="10"/>
       <c r="BH18" s="10"/>
       <c r="BI18" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ18" s="10"/>
       <c r="BK18" s="13"/>
@@ -3163,29 +3223,29 @@
         <v>2</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="13"/>
       <c r="H19" s="10"/>
       <c r="I19" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J19" s="11"/>
       <c r="K19" s="10"/>
       <c r="L19" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
@@ -3193,12 +3253,12 @@
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U19" s="13"/>
       <c r="V19" s="10"/>
       <c r="W19" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X19" s="13"/>
       <c r="Y19" s="10"/>
@@ -3206,7 +3266,7 @@
       <c r="AA19" s="10"/>
       <c r="AB19" s="10"/>
       <c r="AC19" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AD19" s="10"/>
       <c r="AE19" s="10"/>
@@ -3222,12 +3282,12 @@
       <c r="AO19" s="10"/>
       <c r="AP19" s="10"/>
       <c r="AQ19" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AR19" s="10"/>
       <c r="AS19" s="10"/>
       <c r="AT19" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AU19" s="10"/>
       <c r="AV19" s="10"/>
@@ -3237,22 +3297,22 @@
         <v>0</v>
       </c>
       <c r="AZ19" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BA19" s="10"/>
       <c r="BB19" s="10"/>
       <c r="BC19" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BD19" s="10"/>
       <c r="BE19" s="10"/>
       <c r="BF19" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BG19" s="10"/>
       <c r="BH19" s="10"/>
       <c r="BI19" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ19" s="10"/>
       <c r="BK19" s="13"/>
@@ -3282,136 +3342,136 @@
         <v>2</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="10"/>
       <c r="L20" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M20" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N20" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
       <c r="Q20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T20" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="U20" s="13"/>
       <c r="V20" s="10"/>
       <c r="W20" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X20" s="13"/>
       <c r="Y20" s="10"/>
       <c r="Z20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AA20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AB20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC20" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AD20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AF20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AG20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AH20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AI20" s="10"/>
       <c r="AJ20" s="10"/>
       <c r="AK20" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AL20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AM20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AN20" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AO20" s="10"/>
       <c r="AP20" s="10"/>
       <c r="AQ20" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AR20" s="10"/>
       <c r="AS20" s="10"/>
       <c r="AT20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU20" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV20" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW20" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX20" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY20" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ20" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="AU20" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AV20" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AW20" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AX20" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AY20" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AZ20" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="BA20" s="11"/>
       <c r="BB20" s="11"/>
       <c r="BC20" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BD20" s="10"/>
       <c r="BE20" s="10"/>
       <c r="BF20" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BG20" s="10"/>
       <c r="BH20" s="10"/>
       <c r="BI20" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ20" s="10"/>
       <c r="BK20" s="13"/>
@@ -3441,16 +3501,16 @@
         <v>2</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="13" t="s">
-        <v>17</v>
-      </c>
       <c r="E21" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
@@ -3463,7 +3523,7 @@
         <v>1</v>
       </c>
       <c r="N21" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O21" s="10"/>
       <c r="P21" s="10"/>
@@ -3474,7 +3534,7 @@
       <c r="U21" s="10"/>
       <c r="V21" s="10"/>
       <c r="W21" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X21" s="13"/>
       <c r="Y21" s="10"/>
@@ -3490,7 +3550,7 @@
       <c r="AI21" s="11"/>
       <c r="AJ21" s="11"/>
       <c r="AK21" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AL21" s="11"/>
       <c r="AM21" s="12"/>
@@ -3510,7 +3570,7 @@
       <c r="BA21" s="10"/>
       <c r="BB21" s="10"/>
       <c r="BC21" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BD21" s="10"/>
       <c r="BE21" s="10"/>
@@ -3518,7 +3578,7 @@
       <c r="BG21" s="10"/>
       <c r="BH21" s="10"/>
       <c r="BI21" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="BJ21" s="10"/>
       <c r="BK21" s="13"/>
@@ -3548,184 +3608,184 @@
         <v>2</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="N22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="O22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="R22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="S22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="T22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="U22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="V22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="W22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="X22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AI22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AO22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AS22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="BD22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BE22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BH22" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="BI22" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="I22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="L22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="N22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="O22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="P22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="R22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="S22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="T22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="U22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="V22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="W22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="X22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="AL22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AT22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AU22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AV22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AW22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AX22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AY22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AZ22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="BA22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="BB22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="BC22" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="BD22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="BE22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="BF22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="BG22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="BH22" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="BI22" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="BJ22" s="10"/>
       <c r="BK22" s="13"/>

</xml_diff>

<commit_message>
fix physical error in maze
</commit_message>
<xml_diff>
--- a/Labyrinthe.xlsx
+++ b/Labyrinthe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Megaport\Desktop\1ARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A0E22B-4F3A-4E69-9FA6-A2DD512A833E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA656D23-0294-4E1C-B7CD-B4CD15F79A12}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3470" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="17">
   <si>
     <t>DD</t>
   </si>
@@ -544,7 +544,7 @@
   <dimension ref="A1:CE34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="AN10" sqref="AN10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1566,11 +1566,9 @@
         <v>13</v>
       </c>
       <c r="AC7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD7" s="11" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="AD7" s="11"/>
       <c r="AE7" s="10"/>
       <c r="AF7" s="9"/>
       <c r="AG7" s="9"/>
@@ -1702,9 +1700,11 @@
       <c r="Z8" s="9"/>
       <c r="AA8" s="10"/>
       <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
+      <c r="AC8" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="AD8" s="10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="AE8" s="10" t="s">
         <v>4</v>

</xml_diff>